<commit_message>
load ocha to flow, add cli
</commit_message>
<xml_diff>
--- a/product.xlsx
+++ b/product.xlsx
@@ -8,12 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\thamFlowAcc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384A46C7-5836-464D-83AB-BD4161AF7111}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0A1EC6-1750-42AC-A991-82A81E11416D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2B663E49-10EA-4A01-94CD-B862003FF610}"/>
   </bookViews>
   <sheets>
     <sheet name="page365" sheetId="1" r:id="rId1"/>
+    <sheet name="ocha_rice_rama9" sheetId="2" r:id="rId2"/>
+    <sheet name="ocha_vegetable_rama9" sheetId="3" r:id="rId3"/>
+    <sheet name="ocha_rest_chomphon" sheetId="4" r:id="rId4"/>
+    <sheet name="ocha_front_chomphon" sheetId="5" r:id="rId5"/>
+    <sheet name="ocha_rice_sanpatong" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -129,8 +134,533 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Dell</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{228C8615-0825-4481-BFFF-A764A96A6AA8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+ชื่อสินค้าแต่ละที่ page365, ocha, loyverse</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{6D294E03-AF97-4846-9D19-FBEB7E03683B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+เทียบเท่า
+PAGE365 = SKU 
+OCHA = เมนูย่อย</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{A25510FB-FFB0-4CD8-8C60-530B2CA3EA52}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+ProductType:
+1: บริการ
+3: สินค้าไม่นับสต๊อค
+5: สินค้านับสต๊อค</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{85031055-E390-42A5-A01E-0BA48180DA87}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+7: ภาษี 7%
+0: ภาษี 0%
+-1: ยกเว้นภาษี</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Dell</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{EEC94C50-F941-49A2-8EFC-84BB1D997A80}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+ชื่อสินค้าแต่ละที่ page365, ocha, loyverse</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{11C2B00C-E015-4CFF-98E3-94A29AC180A7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+เทียบเท่า
+PAGE365 = SKU 
+OCHA = เมนูย่อย</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{1A792E7C-80AB-4EA1-B2E6-37668B5568C4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+ProductType:
+1: บริการ
+3: สินค้าไม่นับสต๊อค
+5: สินค้านับสต๊อค</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{0E062C33-43F3-416C-B3CA-42B3F91177B8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+7: ภาษี 7%
+0: ภาษี 0%
+-1: ยกเว้นภาษี</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Dell</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{B9AC1F63-7CA4-4231-A02A-56D8BBB3E4FB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+ชื่อสินค้าแต่ละที่ page365, ocha, loyverse</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{C719D672-675C-46DA-BEB4-8B27921E9599}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+เทียบเท่า
+PAGE365 = SKU 
+OCHA = เมนูย่อย</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{F45DAE7E-297A-401E-9EA6-354A29E0C0A0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+ProductType:
+1: บริการ
+3: สินค้าไม่นับสต๊อค
+5: สินค้านับสต๊อค</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{0F176D98-BBC3-498A-BA36-A0D18DF1C344}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+7: ภาษี 7%
+0: ภาษี 0%
+-1: ยกเว้นภาษี</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Dell</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{56129FEE-F7AC-4302-88BA-C6D139AC3958}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+ชื่อสินค้าแต่ละที่ page365, ocha, loyverse</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{57BF5822-20A8-4FFF-B107-67DA0BD36CC3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+เทียบเท่า
+PAGE365 = SKU 
+OCHA = เมนูย่อย</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{A99FDF6B-0B1F-4A98-A03B-98A5015E5F00}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+ProductType:
+1: บริการ
+3: สินค้าไม่นับสต๊อค
+5: สินค้านับสต๊อค</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{3EB5837C-FAFB-41DE-BECA-002F35F607B5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+7: ภาษี 7%
+0: ภาษี 0%
+-1: ยกเว้นภาษี</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Dell</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{3CAB19FC-B4B9-458F-A149-447914BA7875}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+ชื่อสินค้าแต่ละที่ page365, ocha, loyverse</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{A0A8C527-6E31-4B2C-A5C8-CB0226156197}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+เทียบเท่า
+PAGE365 = SKU 
+OCHA = เมนูย่อย</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{81519C1E-F67F-4F8F-8821-885DDB941BB8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+ProductType:
+1: บริการ
+3: สินค้าไม่นับสต๊อค
+5: สินค้านับสต๊อค</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{79089A04-CBC0-437D-931B-72EFA81898F1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+7: ภาษี 7%
+0: ภาษี 0%
+-1: ยกเว้นภาษี</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="33">
   <si>
     <t>vatRate</t>
   </si>
@@ -214,6 +744,21 @@
   </si>
   <si>
     <t>5กก.</t>
+  </si>
+  <si>
+    <t>ข้าวหอมมะลิ 5 กก.</t>
+  </si>
+  <si>
+    <t>5กก</t>
+  </si>
+  <si>
+    <t>ข้าวกล้องเหนียวธรรมชาติ 5 กก</t>
+  </si>
+  <si>
+    <t>ข้าวกล้องธรรมชาติ 5 กก.(ฐธ9)</t>
+  </si>
+  <si>
+    <t>ข้าวหอมมะลิ 5 กก.(ฐธ9)</t>
   </si>
 </sst>
 </file>
@@ -576,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F130F3C-E775-46B0-B969-C84ADC69D298}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -672,7 +1217,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
         <v>22</v>
@@ -686,42 +1231,42 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5">
         <v>5</v>
       </c>
       <c r="G5">
-        <v>7</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -732,19 +1277,377 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>26</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C305091-0D56-4272-9CED-304A82EBAF5A}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.19921875" customWidth="1"/>
+    <col min="2" max="2" width="15.69921875" customWidth="1"/>
+    <col min="3" max="3" width="17.796875" customWidth="1"/>
+    <col min="4" max="5" width="28.296875" customWidth="1"/>
+    <col min="6" max="6" width="15.8984375" customWidth="1"/>
+    <col min="7" max="7" width="15.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB4F6200-A798-40E1-A363-3A93B462AE5D}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.19921875" customWidth="1"/>
+    <col min="2" max="2" width="15.69921875" customWidth="1"/>
+    <col min="3" max="3" width="17.796875" customWidth="1"/>
+    <col min="4" max="5" width="28.296875" customWidth="1"/>
+    <col min="6" max="6" width="15.8984375" customWidth="1"/>
+    <col min="7" max="7" width="15.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B02FE57-70E9-4847-984F-7F9BB9CD3990}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.19921875" customWidth="1"/>
+    <col min="2" max="2" width="15.69921875" customWidth="1"/>
+    <col min="3" max="3" width="17.796875" customWidth="1"/>
+    <col min="4" max="5" width="28.296875" customWidth="1"/>
+    <col min="6" max="6" width="15.8984375" customWidth="1"/>
+    <col min="7" max="7" width="15.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD30406-37C7-49FF-AE1A-BF228BC3BD42}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.19921875" customWidth="1"/>
+    <col min="2" max="2" width="15.69921875" customWidth="1"/>
+    <col min="3" max="3" width="17.796875" customWidth="1"/>
+    <col min="4" max="5" width="28.296875" customWidth="1"/>
+    <col min="6" max="6" width="15.8984375" customWidth="1"/>
+    <col min="7" max="7" width="15.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{693F37E2-0AD2-4797-9670-DBA2CD0887BE}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.19921875" customWidth="1"/>
+    <col min="2" max="2" width="15.69921875" customWidth="1"/>
+    <col min="3" max="3" width="17.796875" customWidth="1"/>
+    <col min="4" max="5" width="28.296875" customWidth="1"/>
+    <col min="6" max="6" width="15.8984375" customWidth="1"/>
+    <col min="7" max="7" width="15.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>